<commit_message>
updated blocking covers all shelves
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Soup GMI KPI template v0.2.xlsx
+++ b/Projects/GMIUS/Data/Soup GMI KPI template v0.2.xlsx
@@ -15,8 +15,7 @@
     <sheet name="Count of" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Blocking" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Adjacency" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Blocking All Shelves" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Result" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Result" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="121">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -120,9 +119,6 @@
     <t xml:space="preserve">Blocking</t>
   </si>
   <si>
-    <t xml:space="preserve">Blocking All Shelves</t>
-  </si>
-  <si>
     <t xml:space="preserve">How is Progresso RTS Light blocked?</t>
   </si>
   <si>
@@ -303,6 +299,9 @@
     <t xml:space="preserve">blocking</t>
   </si>
   <si>
+    <t xml:space="preserve">blocking covers</t>
+  </si>
+  <si>
     <t xml:space="preserve">adj rts o</t>
   </si>
   <si>
@@ -331,9 +330,6 @@
   </si>
   <si>
     <t xml:space="preserve">adj camp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blocking covers</t>
   </si>
   <si>
     <t xml:space="preserve">Result Key</t>
@@ -512,20 +508,20 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.2962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.2777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.2555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.3333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,7 +771,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>10</v>
@@ -806,7 +802,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>29</v>
@@ -823,7 +819,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>29</v>
@@ -840,7 +836,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>29</v>
@@ -857,7 +853,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>29</v>
@@ -874,10 +870,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>10</v>
@@ -891,10 +887,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>10</v>
@@ -908,10 +904,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>10</v>
@@ -925,10 +921,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>10</v>
@@ -942,10 +938,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>10</v>
@@ -959,10 +955,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>10</v>
@@ -976,10 +972,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>10</v>
@@ -993,10 +989,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>10</v>
@@ -1010,10 +1006,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>10</v>
@@ -1027,10 +1023,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>10</v>
@@ -1044,10 +1040,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>10</v>
@@ -1061,10 +1057,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>10</v>
@@ -1078,10 +1074,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>10</v>
@@ -1095,10 +1091,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>10</v>
@@ -1134,12 +1130,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.4481481481482"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.277777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.5259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="121.314814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1147,39 +1143,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1206,9 +1202,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,13 +1212,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,13 +1226,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1263,11 +1259,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.3259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5518518518518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,209 +1271,209 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="F1" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="D7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1504,11 +1500,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.8592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,50 +1512,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1585,19 +1581,19 @@
   <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.4333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.4925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,19 +1601,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G1" s="2"/>
     </row>
@@ -1626,19 +1622,19 @@
         <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,98 +1642,118 @@
         <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1766,12 +1782,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.6555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,19 +1795,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,16 +1815,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>91</v>
@@ -1819,10 +1835,10 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>92</v>
@@ -1833,10 +1849,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>93</v>
@@ -1847,10 +1863,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>93</v>
@@ -1861,10 +1877,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>94</v>
@@ -1875,16 +1891,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="D7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>95</v>
@@ -1895,10 +1911,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>96</v>
@@ -1909,13 +1925,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
@@ -1929,16 +1945,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>98</v>
@@ -1949,13 +1965,13 @@
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>99</v>
@@ -1980,115 +1996,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.85"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.27037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>12</v>
@@ -2096,13 +2041,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>12</v>
@@ -2110,13 +2055,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>12</v>
@@ -2124,13 +2069,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>12</v>
@@ -2141,10 +2086,10 @@
         <v>91</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>12</v>
@@ -2152,13 +2097,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>12</v>
@@ -2166,13 +2111,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>12</v>
@@ -2180,13 +2125,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>12</v>
@@ -2197,10 +2142,10 @@
         <v>92</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>12</v>
@@ -2211,10 +2156,10 @@
         <v>93</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>12</v>
@@ -2225,10 +2170,10 @@
         <v>100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>12</v>
@@ -2239,10 +2184,10 @@
         <v>97</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>12</v>
@@ -2253,10 +2198,10 @@
         <v>98</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>12</v>
@@ -2267,10 +2212,10 @@
         <v>94</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>12</v>
@@ -2281,10 +2226,10 @@
         <v>95</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>12</v>
@@ -2295,10 +2240,10 @@
         <v>96</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>12</v>

</xml_diff>